<commit_message>
Update on 20240322 Part 2
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/Jobs/职业生涯所有工作地点信息汇总.xlsx
+++ b/文档/其他文档/Others/Jobs/职业生涯所有工作地点信息汇总.xlsx
@@ -200,7 +200,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2017.4.17 - 2024.2.29</t>
+    <t>2017.4.17 - 2024.4.16</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -587,7 +587,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -953,7 +953,7 @@
         <v>44</v>
       </c>
       <c r="L9" s="6">
-        <v>2509</v>
+        <v>2556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>